<commit_message>
Development: create maven project
</commit_message>
<xml_diff>
--- a/敏捷开发有关文档/BackLog(Fate).xlsx
+++ b/敏捷开发有关文档/BackLog(Fate).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -200,6 +200,10 @@
   </si>
   <si>
     <t>Notes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该系统为Tss2.0的主系统，并考虑为另外两个系统提供用户分组管理，消息推送的业务接口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -207,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +221,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -243,10 +255,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A14" sqref="A14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -828,7 +846,21 @@
         <v>41</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:G14"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>